<commit_message>
Modified JFK Risk Register. Added approval and suspension/resumption criteria in the documents.
</commit_message>
<xml_diff>
--- a/documentation/softdev/Risk-Register.xlsx
+++ b/documentation/softdev/Risk-Register.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\softdev\apc-softdev-it111-02\documentation\softdev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="116">
   <si>
     <t>Number</t>
   </si>
@@ -69,18 +69,6 @@
     <t>R2</t>
   </si>
   <si>
-    <t xml:space="preserve">Defective Computer </t>
-  </si>
-  <si>
-    <t>One of the computer in the work station doesn't work</t>
-  </si>
-  <si>
-    <t>Inputed Virus</t>
-  </si>
-  <si>
-    <t>Change AntiVirus</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -195,68 +183,203 @@
     <t>R8</t>
   </si>
   <si>
-    <t>Not meeting the deadline for documentation</t>
-  </si>
-  <si>
-    <t>Modifications in the documentation, Delayed submission of documents</t>
-  </si>
-  <si>
-    <t>Revisions on the documentation</t>
-  </si>
-  <si>
-    <t>Antivirus is not effective</t>
-  </si>
-  <si>
-    <t>Division of Work</t>
-  </si>
-  <si>
-    <t>System Errors</t>
-  </si>
-  <si>
-    <t>System doesn't fully run</t>
-  </si>
-  <si>
-    <t>Coding Error</t>
-  </si>
-  <si>
-    <t>Check all the codes for errors</t>
-  </si>
-  <si>
-    <t>Framework used to develop the system</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> I.T. Department will repair the computer by removing the virus and changing the AntiVirus</t>
-  </si>
-  <si>
-    <t>Client Meeting is not regularly held</t>
-  </si>
-  <si>
-    <t>Training</t>
-  </si>
-  <si>
-    <t>Schedule Meeting</t>
-  </si>
-  <si>
-    <t>Unfamiliarity of the framework used</t>
-  </si>
-  <si>
-    <t>Changes Made</t>
-  </si>
-  <si>
-    <t>Employees will be trained / Hiring someone who is knowledgable in that field</t>
-  </si>
-  <si>
-    <t>Project Leader and Team  Members will divide the work</t>
-  </si>
-  <si>
-    <t>Debugging</t>
+    <t>Technical Risk</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project may not be able </t>
+  </si>
+  <si>
+    <t>to continue</t>
+  </si>
+  <si>
+    <t>I.T. Dept.</t>
+  </si>
+  <si>
+    <t>development</t>
+  </si>
+  <si>
+    <t>Hosting ended</t>
+  </si>
+  <si>
+    <t>Hosting of APC ends after the finals</t>
+  </si>
+  <si>
+    <t>P1: buy the hosting server</t>
+  </si>
+  <si>
+    <t>P2: look for free hosting server</t>
+  </si>
+  <si>
+    <t>Finance Dept. &amp; I.T. Dept.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Will use the company owner's another </t>
+  </si>
+  <si>
+    <t>system's hosting server</t>
+  </si>
+  <si>
+    <t>Documents not finished</t>
+  </si>
+  <si>
+    <t>on time</t>
+  </si>
+  <si>
+    <t>Creating documents not finished on time for static testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Many revisions and </t>
+  </si>
+  <si>
+    <t>wrong time management</t>
+  </si>
+  <si>
+    <t>May fail the static testing</t>
+  </si>
+  <si>
+    <t>P2: extend time on doing the documents</t>
+  </si>
+  <si>
+    <t>to meet the submission time</t>
+  </si>
+  <si>
+    <t>finished</t>
+  </si>
+  <si>
+    <t>P1: submit only what the team has</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I.T. Department will extend time to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">finish doing the documents for static </t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not finishing the </t>
+  </si>
+  <si>
+    <t xml:space="preserve">system before the </t>
+  </si>
+  <si>
+    <t>finals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Donation and Shopping Cart Modules are still under </t>
+  </si>
+  <si>
+    <t>for the online transaction</t>
+  </si>
+  <si>
+    <t>P2: Hire programmer</t>
+  </si>
+  <si>
+    <t>P1: abort using extension and find</t>
+  </si>
+  <si>
+    <t>another way.</t>
+  </si>
+  <si>
+    <t>Deployment of the system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">may be extended </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC1: Developers are trying </t>
+  </si>
+  <si>
+    <t>to use paypal extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC2: One of the </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prgrammers could not </t>
+  </si>
+  <si>
+    <t>because of health issues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just redirect the site to paypal's </t>
+  </si>
+  <si>
+    <t xml:space="preserve">payment form and extend working </t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>No Maintenance</t>
+  </si>
+  <si>
+    <t>No maintenance for the system after deployment</t>
+  </si>
+  <si>
+    <t>Didn't include on project's</t>
+  </si>
+  <si>
+    <t>planning phase</t>
+  </si>
+  <si>
+    <t>Owner may not be updated</t>
+  </si>
+  <si>
+    <t>on what's going on with the</t>
+  </si>
+  <si>
+    <t>with the system</t>
+  </si>
+  <si>
+    <t>include it already on the project's plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revise cost project planning and </t>
+  </si>
+  <si>
+    <t>analysis documents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client meeting not </t>
+  </si>
+  <si>
+    <t>conducted</t>
+  </si>
+  <si>
+    <t>Meeting with the client not performed</t>
+  </si>
+  <si>
+    <t>I.T.Dept</t>
+  </si>
+  <si>
+    <t>Client cancels the meeting</t>
+  </si>
+  <si>
+    <t>Updates and progress not</t>
+  </si>
+  <si>
+    <t>informed to the client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set another date and time for the </t>
+  </si>
+  <si>
+    <t>meeting</t>
+  </si>
+  <si>
+    <t>Client meeting rescheduled</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,13 +396,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -287,6 +403,20 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -328,23 +458,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -626,236 +752,589 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" style="6" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="48.5703125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="30.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="51.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="38.140625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="30.28515625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="6"/>
+    <col min="12" max="12" width="35.85546875" style="6" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="M1"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="9">
+        <v>3</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4"/>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="9">
+        <v>2</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="M5"/>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="M7"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="9">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C10" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="M10"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="M11"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12"/>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13"/>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="M14"/>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="M15"/>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="M16"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18"/>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19"/>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20"/>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="9">
+        <v>5</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="J21" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="7">
-        <v>5</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="7">
-        <v>3</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="7">
-        <v>2</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="7">
-        <v>1</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" s="8"/>
-    </row>
-    <row r="7" spans="1:12" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-    </row>
-    <row r="8" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="K21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="M21"/>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -887,7 +1366,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -936,10 +1415,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -950,24 +1429,24 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -980,111 +1459,111 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="L6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
       <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
         <v>25</v>
       </c>
-      <c r="D8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" t="s">
         <v>27</v>
-      </c>
-      <c r="F8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
         <v>30</v>
-      </c>
-      <c r="G9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" t="s">
         <v>36</v>
       </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="J10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" t="s">
         <v>37</v>
-      </c>
-      <c r="F10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L10" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>